<commit_message>
Last update before deadline lol
</commit_message>
<xml_diff>
--- a/Resultaten.xlsx
+++ b/Resultaten.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joep\mPWS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{192C1FE7-C14A-4ED2-92F2-A4B77FB42156}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F21821D7-0A00-4C6C-9066-E4CADB36948B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="no_april" sheetId="1" r:id="rId1"/>
@@ -1523,7 +1523,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1544,6 +1544,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1619,18 +1624,7 @@
     <cellStyle name="Check Cell" xfId="2" builtinId="23"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1746,20 +1740,6 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
           <c:cat>
             <c:strRef>
               <c:f>no_april!$D$2:$D$241</c:f>
@@ -3242,20 +3222,6 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
           <c:cat>
             <c:strRef>
               <c:f>no_april!$D$2:$D$241</c:f>
@@ -11896,20 +11862,6 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
           <c:cat>
             <c:strRef>
               <c:f>no_april!$D$2:$D$241</c:f>
@@ -13392,20 +13344,6 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
           <c:cat>
             <c:strRef>
               <c:f>no_april!$D$2:$D$241</c:f>
@@ -17888,10 +17826,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L241"/>
+  <dimension ref="A1:AF241"/>
   <sheetViews>
-    <sheetView topLeftCell="A157" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L32" sqref="L32"/>
+    <sheetView tabSelected="1" topLeftCell="T1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AF6" sqref="AF6:AF21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -17904,7 +17842,7 @@
     <col min="6" max="1025" width="11.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -17921,7 +17859,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -17939,7 +17877,7 @@
         <v>0.53</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -17957,7 +17895,7 @@
         <v>1.0489999999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -17975,7 +17913,7 @@
         <v>31.526000000000003</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -17993,7 +17931,7 @@
         <v>32.802999999999997</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -18010,8 +17948,9 @@
         <f t="shared" si="0"/>
         <v>-1.1200000000000001</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="AF6" s="1"/>
+    </row>
+    <row r="7" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -18028,8 +17967,9 @@
         <f t="shared" si="0"/>
         <v>0.54199999999999982</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="AF7" s="1"/>
+    </row>
+    <row r="8" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
@@ -18046,8 +17986,9 @@
         <f t="shared" si="0"/>
         <v>-0.95300000000000029</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="AF8" s="1"/>
+    </row>
+    <row r="9" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
@@ -18064,8 +18005,9 @@
         <f t="shared" si="0"/>
         <v>-1.819</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="AF9" s="1"/>
+    </row>
+    <row r="10" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
@@ -18082,8 +18024,9 @@
         <f t="shared" si="0"/>
         <v>0.27800000000000002</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="AF10" s="1"/>
+    </row>
+    <row r="11" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
@@ -18100,8 +18043,9 @@
         <f t="shared" si="0"/>
         <v>1.5070000000000001</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="AF11" s="1"/>
+    </row>
+    <row r="12" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>22</v>
       </c>
@@ -18118,8 +18062,9 @@
         <f t="shared" si="0"/>
         <v>3.1530000000000005</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="AF12" s="1"/>
+    </row>
+    <row r="13" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>24</v>
       </c>
@@ -18136,8 +18081,9 @@
         <f t="shared" si="0"/>
         <v>-5.593</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="AF13" s="1"/>
+    </row>
+    <row r="14" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>26</v>
       </c>
@@ -18154,8 +18100,9 @@
         <f t="shared" si="0"/>
         <v>-3.8129999999999988</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="AF14" s="1"/>
+    </row>
+    <row r="15" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>28</v>
       </c>
@@ -18172,8 +18119,9 @@
         <f t="shared" si="0"/>
         <v>-9.2000000000000526E-2</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="AF15" s="1"/>
+    </row>
+    <row r="16" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>30</v>
       </c>
@@ -18190,8 +18138,9 @@
         <f t="shared" si="0"/>
         <v>-2.5640000000000001</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="AF16" s="1"/>
+    </row>
+    <row r="17" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>32</v>
       </c>
@@ -18208,8 +18157,9 @@
         <f t="shared" si="0"/>
         <v>0.2799999999999998</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="AF17" s="1"/>
+    </row>
+    <row r="18" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>34</v>
       </c>
@@ -18226,8 +18176,9 @@
         <f t="shared" si="0"/>
         <v>2.004</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="AF18" s="1"/>
+    </row>
+    <row r="19" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>36</v>
       </c>
@@ -18244,8 +18195,9 @@
         <f t="shared" si="0"/>
         <v>0.23599999999999999</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="AF19" s="1"/>
+    </row>
+    <row r="20" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>38</v>
       </c>
@@ -18262,8 +18214,9 @@
         <f t="shared" si="0"/>
         <v>-4.423</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="AF20" s="1"/>
+    </row>
+    <row r="21" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>40</v>
       </c>
@@ -18280,8 +18233,9 @@
         <f t="shared" si="0"/>
         <v>-11.381</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="AF21" s="1"/>
+    </row>
+    <row r="22" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>42</v>
       </c>
@@ -18299,7 +18253,7 @@
         <v>-3.7779999999999996</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>44</v>
       </c>
@@ -18317,7 +18271,7 @@
         <v>-3.4010000000000007</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>46</v>
       </c>
@@ -18335,7 +18289,7 @@
         <v>-1.7240000000000002</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>48</v>
       </c>
@@ -18353,7 +18307,7 @@
         <v>3.3629999999999995</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>50</v>
       </c>
@@ -18371,7 +18325,7 @@
         <v>9.6959999999999997</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>52</v>
       </c>
@@ -18389,7 +18343,7 @@
         <v>13.344999999999999</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>54</v>
       </c>
@@ -18407,7 +18361,7 @@
         <v>-2.6999999999999247E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>56</v>
       </c>
@@ -18425,7 +18379,7 @@
         <v>-3.6110000000000007</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>58</v>
       </c>
@@ -18443,7 +18397,7 @@
         <v>-10.782</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:32" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>60</v>
       </c>
@@ -18461,7 +18415,7 @@
         <v>-4.2910000000000004</v>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:32" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>62</v>
       </c>
@@ -22256,6 +22210,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
@@ -22270,7 +22225,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N241"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="N32" sqref="N32"/>
     </sheetView>
   </sheetViews>
@@ -26645,7 +26600,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:N241"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="M29" sqref="M29:N30"/>
     </sheetView>
   </sheetViews>
@@ -31021,7 +30976,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:N241"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="M36" sqref="M36"/>
     </sheetView>
   </sheetViews>
@@ -35397,7 +35352,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF9B5EFF-FF0F-41CF-A522-DFB93752895E}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>

</xml_diff>